<commit_message>
Finalise supplementary files for review
</commit_message>
<xml_diff>
--- a/vignettes/supplement_files/sfile_S4.xlsx
+++ b/vignettes/supplement_files/sfile_S4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlotte\Documents\candidaev\vignettes\supplement_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA89E7B9-CFC8-46C6-8730-25319CB25052}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF4360A-4204-40B5-8047-ACCAFFDF6601}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,12 +18,18 @@
     <sheet name="Figure 7A" sheetId="3" r:id="rId3"/>
     <sheet name="Figure 7B" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Figure 5A'!$A$2:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Figure 5B'!$A$2:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Figure 7A'!$A$2:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Figure 7B'!$A$2:$G$2</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="85">
   <si>
     <t>DAY Y</t>
   </si>
@@ -266,6 +272,18 @@
   </si>
   <si>
     <t>AGE3 LTP1 DOA1 GCA1;GCA2 orf19.1514 HPT1 orf19.1785 orf19.1626 GTT11 orf19.7357 HRT2 UAP1 EBP1 SEC27 APA2 orf19.6559 ADE1 TRP2 orf19.4395 orf19.7322 CDC11 orf19.2965 PMI1 CDC10 CYC1 orf19.3515 orf19.1815 GLC7 HSM3 OSM1 ARO7 orf19.2304 CCT2 SUP35 orf19.1946 WRS1 NHP2 PFY1 GSY1 HMT1 SVF1 orf19.338 TRR1 orf19.4248 TIF34 orf19.3938 orf19.4633 POL30 orf19.4816 EIF4E FRS2 DAK2 SAM2 ACT1 ERG10 orf19.2175 ASN1 LYS9 CAR2 PYC2 ADH1 GLN1 FDH3 TSA1;TSA1B;TSA1B PMM1 PDC11 YHB1 ADE6 SIS1 TAL1 CCP1 orf19.3915 APT1 RPP1A TPI1 FBA1</t>
+  </si>
+  <si>
+    <t>This sheet contains lists of significantly enriched or exclusive WCL proteins in each Venn partition shown in Figure 7B.</t>
+  </si>
+  <si>
+    <t>This sheet contains lists of significantly enriched or exclusive EV proteins in each Venn partition shown in Figure 7A.</t>
+  </si>
+  <si>
+    <t>This sheet contains lists of WCL proteins in each Venn partition shown in Figure 5B.</t>
+  </si>
+  <si>
+    <t>This sheet contains lists of EV proteins in each Venn partition shown in Figure 5A.</t>
   </si>
 </sst>
 </file>
@@ -658,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -671,6 +689,11 @@
     <col min="7" max="7" width="86.7265625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
@@ -1040,6 +1063,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:G2" xr:uid="{6D07AF27-C3C5-43F0-8103-39AF87B1F990}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
@@ -1047,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:G17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1060,6 +1084,11 @@
     <col min="7" max="7" width="86.7265625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
@@ -1429,16 +1458,17 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:G2" xr:uid="{2E12EF0C-D5B7-47FF-A068-C98172321464}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:G17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1448,6 +1478,11 @@
     <col min="7" max="7" width="86.7265625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+    </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
@@ -1817,16 +1852,17 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:G2" xr:uid="{E428ADF1-FAA3-47C7-A02D-5C5B15A49733}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A2:G17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1836,6 +1872,11 @@
     <col min="7" max="7" width="86.7265625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
@@ -2202,6 +2243,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:G2" xr:uid="{67AC456A-6B95-415F-A1A5-37F87F511AC1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>